<commit_message>
Add software to the metadata
</commit_message>
<xml_diff>
--- a/tests/resources/metadata_files/EVA_Submission_v2.0_cpombe.xlsx
+++ b/tests/resources/metadata_files/EVA_Submission_v2.0_cpombe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-integration-tests/tests/resources/metadata_spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-integration-tests/tests/resources/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CA6DB4-43E9-E14A-89EC-A38C0157DA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3150CB7C-7802-0A4C-B8B1-0C52634070EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="560">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -1901,6 +1901,9 @@
   </si>
   <si>
     <t>vcf_file_ASM294v2.vcf</t>
+  </si>
+  <si>
+    <t>BWA,GATK,another one</t>
   </si>
 </sst>
 </file>
@@ -2474,17 +2477,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2498,17 +2492,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2785,8 +2788,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="67"/>
-      <c r="B1" s="67"/>
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -2795,10 +2798,10 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="70"/>
+      <c r="B2" s="67"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2807,10 +2810,10 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="71"/>
+      <c r="B3" s="68"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2819,10 +2822,10 @@
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="72"/>
+      <c r="B4" s="69"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2831,10 +2834,10 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="73"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -2867,8 +2870,8 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
-      <c r="B8" s="67"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -2877,10 +2880,10 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="68"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -2889,8 +2892,8 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="67"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -2899,10 +2902,10 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="69"/>
+      <c r="B11" s="73"/>
     </row>
     <row r="12" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
@@ -2954,28 +2957,28 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="66"/>
+      <c r="B19" s="71"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="66"/>
+      <c r="B20" s="71"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="66"/>
+      <c r="B21" s="71"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="66"/>
+      <c r="B22" s="71"/>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
@@ -2984,11 +2987,6 @@
   </sheetData>
   <sheetProtection password="E50B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
@@ -2997,6 +2995,11 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5165,8 +5168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5248,6 +5251,9 @@
       </c>
       <c r="E2" t="s">
         <v>554</v>
+      </c>
+      <c r="H2" t="s">
+        <v>559</v>
       </c>
       <c r="M2" s="30"/>
     </row>
@@ -5770,7 +5776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -5800,15 +5806,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="74" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="75"/>
       <c r="D1" s="42" t="s">
         <v>196</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="75" t="s">
         <v>197</v>
       </c>
       <c r="F1" s="42" t="s">
@@ -5858,63 +5864,63 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" s="48"/>
       <c r="B2" s="49"/>
-      <c r="C2" s="77"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="50"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="75" t="s">
+      <c r="E2" s="75"/>
+      <c r="F2" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="74" t="s">
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74" t="s">
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="75" t="s">
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75" t="s">
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="76"/>
+      <c r="W2" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="75" t="s">
+      <c r="X2" s="76"/>
+      <c r="Y2" s="76"/>
+      <c r="Z2" s="76" t="s">
         <v>148</v>
       </c>
-      <c r="AA2" s="75"/>
-      <c r="AB2" s="75"/>
-      <c r="AC2" s="75"/>
-      <c r="AD2" s="75"/>
-      <c r="AE2" s="75"/>
-      <c r="AF2" s="75"/>
-      <c r="AG2" s="75"/>
-      <c r="AH2" s="75"/>
-      <c r="AI2" s="75"/>
-      <c r="AJ2" s="75" t="s">
+      <c r="AA2" s="76"/>
+      <c r="AB2" s="76"/>
+      <c r="AC2" s="76"/>
+      <c r="AD2" s="76"/>
+      <c r="AE2" s="76"/>
+      <c r="AF2" s="76"/>
+      <c r="AG2" s="76"/>
+      <c r="AH2" s="76"/>
+      <c r="AI2" s="76"/>
+      <c r="AJ2" s="76" t="s">
         <v>169</v>
       </c>
-      <c r="AK2" s="75"/>
-      <c r="AL2" s="75"/>
-      <c r="AM2" s="75"/>
-      <c r="AN2" s="75"/>
-      <c r="AO2" s="75"/>
-      <c r="AP2" s="75"/>
-      <c r="AQ2" s="75"/>
-      <c r="AR2" s="75"/>
-      <c r="AS2" s="75"/>
+      <c r="AK2" s="76"/>
+      <c r="AL2" s="76"/>
+      <c r="AM2" s="76"/>
+      <c r="AN2" s="76"/>
+      <c r="AO2" s="76"/>
+      <c r="AP2" s="76"/>
+      <c r="AQ2" s="76"/>
+      <c r="AR2" s="76"/>
+      <c r="AS2" s="76"/>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A3" s="51" t="s">
@@ -5923,11 +5929,11 @@
       <c r="B3" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="77"/>
+      <c r="C3" s="75"/>
       <c r="D3" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="77"/>
+      <c r="E3" s="75"/>
       <c r="F3" s="53" t="s">
         <v>106</v>
       </c>
@@ -6093,16 +6099,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Z2:AI2"/>
+    <mergeCell ref="AJ2:AS2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F2:K2"/>
     <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="Z2:AI2"/>
-    <mergeCell ref="AJ2:AS2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Analysis alias" prompt="Must match an analysis alias provided in the &quot;ANALYSIS&quot; sheet_x000a_Multiple entries can be separated with a comma_x000a_e.g. analysis1,analysis2" sqref="A3" xr:uid="{00000000-0002-0000-0700-000000000000}">

</xml_diff>